<commit_message>
Oh yeah, I'm the best.
</commit_message>
<xml_diff>
--- a/SimpleCombat/Assets/CombatModule/cards/Card Stats.xlsx
+++ b/SimpleCombat/Assets/CombatModule/cards/Card Stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Card Name</t>
   </si>
@@ -67,6 +67,45 @@
   </si>
   <si>
     <t>speedy</t>
+  </si>
+  <si>
+    <t>wild fred</t>
+  </si>
+  <si>
+    <t>super armor guy</t>
+  </si>
+  <si>
+    <t>wimpy</t>
+  </si>
+  <si>
+    <t>Ninja</t>
+  </si>
+  <si>
+    <t>Flame man</t>
+  </si>
+  <si>
+    <t>WaterDude</t>
+  </si>
+  <si>
+    <t>Guru</t>
+  </si>
+  <si>
+    <t>someone</t>
+  </si>
+  <si>
+    <t>winner</t>
+  </si>
+  <si>
+    <t>health n armor</t>
+  </si>
+  <si>
+    <t>air man</t>
+  </si>
+  <si>
+    <t>swordsman</t>
+  </si>
+  <si>
+    <t>Artist</t>
   </si>
 </sst>
 </file>
@@ -405,20 +444,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" customWidth="1"/>
     <col min="2" max="2" width="9.21875" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+    <col min="16" max="16" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,134 +479,524 @@
       <c r="D1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>28</v>
+      </c>
+      <c r="J3">
+        <v>35</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>25</v>
+      </c>
+      <c r="M3">
+        <v>22</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>25</v>
+      </c>
+      <c r="P3">
+        <v>24</v>
+      </c>
+      <c r="Q3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>90</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>52</v>
+      </c>
+      <c r="J4">
+        <v>55</v>
+      </c>
+      <c r="K4">
+        <v>30</v>
+      </c>
+      <c r="L4">
+        <v>55</v>
+      </c>
+      <c r="M4">
+        <v>58</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>55</v>
+      </c>
+      <c r="P4">
+        <v>56</v>
+      </c>
+      <c r="Q4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+      <c r="O5">
+        <v>14</v>
+      </c>
+      <c r="P5">
+        <v>16</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>37</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>26</v>
+      </c>
+      <c r="J6">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>30</v>
+      </c>
+      <c r="M6">
+        <v>32</v>
+      </c>
+      <c r="N6">
+        <v>28</v>
+      </c>
+      <c r="O6">
+        <v>26</v>
+      </c>
+      <c r="P6">
+        <v>42</v>
+      </c>
+      <c r="Q6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>75</v>
+      </c>
+      <c r="G7">
+        <v>102</v>
+      </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>35</v>
+      </c>
+      <c r="K7">
+        <v>40</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="M7">
+        <v>52</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
+      <c r="O7">
+        <v>38</v>
+      </c>
+      <c r="P7">
+        <v>62</v>
+      </c>
+      <c r="Q7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>10</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
         <v>4</v>
       </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>3</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -571,8 +1009,47 @@
       <c r="D11">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>85</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>20</v>
+      </c>
+      <c r="I11">
+        <v>55</v>
+      </c>
+      <c r="J11">
+        <v>65</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <v>50</v>
+      </c>
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11">
+        <v>60</v>
+      </c>
+      <c r="P11">
+        <v>40</v>
+      </c>
+      <c r="Q11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -580,13 +1057,52 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>15</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>40</v>
+      </c>
+      <c r="I12">
+        <v>25</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>50</v>
+      </c>
+      <c r="L12">
+        <v>30</v>
+      </c>
+      <c r="M12">
+        <v>30</v>
+      </c>
+      <c r="N12">
+        <v>15</v>
+      </c>
+      <c r="O12">
+        <v>30</v>
+      </c>
+      <c r="P12">
+        <v>20</v>
+      </c>
+      <c r="Q12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -594,25 +1110,117 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
+        <f xml:space="preserve"> SUM(B2:B4)/6 + SUM(B5:B7)/6 + SUM(B8:B10)/6 + SUM(B11:B12)/5 + B13</f>
         <v>50</v>
       </c>
       <c r="C14">
-        <f>SUM(C2:C10)/2 + SUM(C11 + C12)/5 + C13</f>
-        <v>50.5</v>
+        <f xml:space="preserve"> SUM(C2:C4)/6 + SUM(C5:C7)/6 + SUM(C8:C10)/6 + SUM(C11:C12)/5 + C13</f>
+        <v>50</v>
       </c>
       <c r="D14">
-        <f>SUM(D2:D10)/2 + SUM(D11:D12)/5 + D13</f>
+        <f xml:space="preserve"> SUM(D2:D4)/6 + SUM(D5:D7)/6 + SUM(D8:D10)/6 + SUM(D11:D12)/5 + D13</f>
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <f xml:space="preserve"> SUM(E2:E4)/6 + SUM(E5:E7)/6 + SUM(E8:E10)/6 + SUM(E11:E12)/5 + E13</f>
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:J14" si="0" xml:space="preserve"> SUM(F2:F4)/6 + SUM(F5:F7)/6 + SUM(F8:F10)/6 + SUM(F11:F12)/5 + F13</f>
+        <v>50</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="K14" si="1" xml:space="preserve"> SUM(K2:K4)/6 + SUM(K5:K7)/6 + SUM(K8:K10)/6 + SUM(K11:K12)/5 + K13</f>
+        <v>50</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14" si="2" xml:space="preserve"> SUM(L2:L4)/6 + SUM(L5:L7)/6 + SUM(L8:L10)/6 + SUM(L11:L12)/5 + L13</f>
+        <v>50</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14" si="3" xml:space="preserve"> SUM(M2:M4)/6 + SUM(M5:M7)/6 + SUM(M8:M10)/6 + SUM(M11:M12)/5 + M13</f>
+        <v>50</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14" si="4" xml:space="preserve"> SUM(N2:N4)/6 + SUM(N5:N7)/6 + SUM(N8:N10)/6 + SUM(N11:N12)/5 + N13</f>
+        <v>50</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ref="O14" si="5" xml:space="preserve"> SUM(O2:O4)/6 + SUM(O5:O7)/6 + SUM(O8:O10)/6 + SUM(O11:O12)/5 + O13</f>
+        <v>50</v>
+      </c>
+      <c r="P14">
+        <f t="shared" ref="P14:Q14" si="6" xml:space="preserve"> SUM(P2:P4)/6 + SUM(P5:P7)/6 + SUM(P8:P10)/6 + SUM(P11:P12)/5 + P13</f>
+        <v>50</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
     </row>

</xml_diff>